<commit_message>
Edited data file with more songs
</commit_message>
<xml_diff>
--- a/Song Correlation.xlsx
+++ b/Song Correlation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>Alice in Chains - Rooster</t>
   </si>
@@ -49,13 +49,40 @@
   </si>
   <si>
     <t>Nirvana - Heart Shaped Box</t>
+  </si>
+  <si>
+    <t>Gloria Gaynor - I Will Survive</t>
+  </si>
+  <si>
+    <t>J Balvin - Ay Vamos</t>
+  </si>
+  <si>
+    <t>Ozuna - Dile Que Tu Me Quieres</t>
+  </si>
+  <si>
+    <t>The Smashing Pumpkins - Today</t>
+  </si>
+  <si>
+    <t>Ghostbusters Theme Song</t>
+  </si>
+  <si>
+    <t>Huey Lewis and The News - I Want a New Drug</t>
+  </si>
+  <si>
+    <t>Kool &amp; The Gang - Get Down On It</t>
+  </si>
+  <si>
+    <t>Weezer - Undone - The Sweater Song</t>
+  </si>
+  <si>
+    <t>The All American Rejects - Move Along</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -65,16 +92,33 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -82,13 +126,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,13 +434,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" customWidth="1"/>
@@ -389,7 +454,7 @@
     <col min="11" max="11" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
@@ -421,7 +486,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -456,7 +521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,7 +554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -520,7 +585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -549,7 +614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -573,7 +638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -594,7 +659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -611,7 +676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -625,7 +690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -636,7 +701,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -644,7 +709,53 @@
         <v>4</v>
       </c>
     </row>
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A13" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A16" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A17" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A18" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A19" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A20" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated song data (Song Correlation 2.0 contains binary data instead of Multi-Class)
</commit_message>
<xml_diff>
--- a/Song Correlation.xlsx
+++ b/Song Correlation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
   <si>
     <t>Alice in Chains - Rooster</t>
   </si>
@@ -63,19 +63,61 @@
     <t>The Smashing Pumpkins - Today</t>
   </si>
   <si>
-    <t>Ghostbusters Theme Song</t>
-  </si>
-  <si>
-    <t>Huey Lewis and The News - I Want a New Drug</t>
-  </si>
-  <si>
     <t>Kool &amp; The Gang - Get Down On It</t>
   </si>
   <si>
     <t>Weezer - Undone - The Sweater Song</t>
   </si>
   <si>
-    <t>The All American Rejects - Move Along</t>
+    <t>Kesha - Tik Tok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Katy Perry - California Girls </t>
+  </si>
+  <si>
+    <t>The Police - Roxanne</t>
+  </si>
+  <si>
+    <t>Ed Sheeran - Thinking Out Loud</t>
+  </si>
+  <si>
+    <t>Bruno Mars - Locked Out Of Heaven</t>
+  </si>
+  <si>
+    <t>Marvin Gaye - Let's Get It On</t>
+  </si>
+  <si>
+    <t>Social Casualty - 5 Seconds Of Summer</t>
+  </si>
+  <si>
+    <t>Fall Out Boy - Sugar, We're Goin Down</t>
+  </si>
+  <si>
+    <t>Panic At The Disco - This Is Gospel</t>
+  </si>
+  <si>
+    <t>Meghan Trainor - Dear Future Husband</t>
+  </si>
+  <si>
+    <t>Olly Murs - Dance With Me Tonight</t>
+  </si>
+  <si>
+    <t>Dion - Runaround Sue</t>
+  </si>
+  <si>
+    <t>Lagy Gaga - Born This Way</t>
+  </si>
+  <si>
+    <t>Madonna - Express Yourself</t>
+  </si>
+  <si>
+    <t>Kool &amp; The Gang - Get Down On it</t>
+  </si>
+  <si>
+    <t>Weezer - Undone -- The Sweater Song</t>
+  </si>
+  <si>
+    <t>The Pixies - Where Is My Mind</t>
   </si>
 </sst>
 </file>
@@ -145,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -154,6 +196,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:AG32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -454,7 +497,7 @@
     <col min="11" max="11" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1">
+    <row r="1" spans="1:33" ht="15.75" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
@@ -485,8 +528,71 @@
       <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1">
+      <c r="L1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>18</v>
+      </c>
+      <c r="W1" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -520,8 +626,72 @@
       <c r="K2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1">
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="Q2">
+        <v>3</v>
+      </c>
+      <c r="R2">
+        <v>3</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>3</v>
+      </c>
+      <c r="Z2">
+        <v>3</v>
+      </c>
+      <c r="AA2">
+        <v>3</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="1"/>
+    </row>
+    <row r="3" spans="1:33" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -553,8 +723,72 @@
       <c r="K3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1">
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+      <c r="Q3">
+        <v>3</v>
+      </c>
+      <c r="R3">
+        <v>3</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>3</v>
+      </c>
+      <c r="Z3">
+        <v>3</v>
+      </c>
+      <c r="AA3">
+        <v>3</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="1"/>
+    </row>
+    <row r="4" spans="1:33" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -584,8 +818,72 @@
       <c r="K4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1">
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <v>4</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>2</v>
+      </c>
+      <c r="Q4">
+        <v>2</v>
+      </c>
+      <c r="R4">
+        <v>2</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>2</v>
+      </c>
+      <c r="V4">
+        <v>2</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="1"/>
+    </row>
+    <row r="5" spans="1:33" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -613,8 +911,72 @@
       <c r="K5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1">
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="M5">
+        <v>4</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>2</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5">
+        <v>2</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>2</v>
+      </c>
+      <c r="V5">
+        <v>2</v>
+      </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>1</v>
+      </c>
+      <c r="AG5" s="1"/>
+    </row>
+    <row r="6" spans="1:33" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -637,8 +999,72 @@
       <c r="K6" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1">
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="1"/>
+    </row>
+    <row r="7" spans="1:33" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -658,8 +1084,72 @@
       <c r="K7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1">
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="1"/>
+    </row>
+    <row r="8" spans="1:33" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -675,8 +1165,72 @@
       <c r="K8" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1">
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>3</v>
+      </c>
+      <c r="Q8">
+        <v>2</v>
+      </c>
+      <c r="R8">
+        <v>3</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <v>3</v>
+      </c>
+      <c r="Z8">
+        <v>3</v>
+      </c>
+      <c r="AA8">
+        <v>3</v>
+      </c>
+      <c r="AB8">
+        <v>1</v>
+      </c>
+      <c r="AC8">
+        <v>1</v>
+      </c>
+      <c r="AD8">
+        <v>1</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="1"/>
+    </row>
+    <row r="9" spans="1:33" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -689,8 +1243,72 @@
       <c r="K9" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1">
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>4</v>
+      </c>
+      <c r="Q9">
+        <v>3</v>
+      </c>
+      <c r="R9">
+        <v>4</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+      <c r="V9">
+        <v>1</v>
+      </c>
+      <c r="W9">
+        <v>1</v>
+      </c>
+      <c r="X9">
+        <v>1</v>
+      </c>
+      <c r="Y9">
+        <v>3</v>
+      </c>
+      <c r="Z9">
+        <v>3</v>
+      </c>
+      <c r="AA9">
+        <v>3</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="1"/>
+    </row>
+    <row r="10" spans="1:33" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -700,58 +1318,946 @@
       <c r="K10" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>4</v>
+      </c>
+      <c r="O10">
+        <v>4</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="1"/>
+    </row>
+    <row r="11" spans="1:33" ht="15.75" customHeight="1" thickBot="1">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="K11" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>4</v>
+      </c>
+      <c r="O11">
+        <v>4</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="1"/>
+    </row>
+    <row r="12" spans="1:33" ht="15.75" customHeight="1" thickBot="1">
       <c r="A12" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+        <v>14</v>
+      </c>
+      <c r="L12">
+        <v>4</v>
+      </c>
+      <c r="M12">
+        <v>4</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>2</v>
+      </c>
+      <c r="Q12">
+        <v>2</v>
+      </c>
+      <c r="R12">
+        <v>2</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>2</v>
+      </c>
+      <c r="V12">
+        <v>2</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <v>0</v>
+      </c>
+      <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="2"/>
+    </row>
+    <row r="13" spans="1:33" ht="15.75" customHeight="1" thickBot="1">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+      <c r="M13">
+        <v>4</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>2</v>
+      </c>
+      <c r="V13">
+        <v>2</v>
+      </c>
+      <c r="W13">
+        <v>1</v>
+      </c>
+      <c r="X13">
+        <v>1</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
+        <v>0</v>
+      </c>
+      <c r="AF13">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="2"/>
+    </row>
+    <row r="14" spans="1:33" ht="15.75" customHeight="1" thickBot="1">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+      <c r="N14">
+        <v>4</v>
+      </c>
+      <c r="O14">
+        <v>4</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14">
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <v>0</v>
+      </c>
+      <c r="AE14">
+        <v>0</v>
+      </c>
+      <c r="AF14">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="2"/>
+    </row>
+    <row r="15" spans="1:33" ht="15.75" customHeight="1" thickBot="1">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+      <c r="O15">
+        <v>4</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <v>0</v>
+      </c>
+      <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="2"/>
+    </row>
+    <row r="16" spans="1:33" ht="15.75" customHeight="1" thickBot="1">
       <c r="A16" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="15.75" customHeight="1" thickBot="1">
+        <v>15</v>
+      </c>
+      <c r="P16">
+        <v>4</v>
+      </c>
+      <c r="Q16">
+        <v>4</v>
+      </c>
+      <c r="R16">
+        <v>4</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>1</v>
+      </c>
+      <c r="V16">
+        <v>1</v>
+      </c>
+      <c r="W16">
+        <v>1</v>
+      </c>
+      <c r="X16">
+        <v>1</v>
+      </c>
+      <c r="Y16">
+        <v>3</v>
+      </c>
+      <c r="Z16">
+        <v>3</v>
+      </c>
+      <c r="AA16">
+        <v>3</v>
+      </c>
+      <c r="AB16">
+        <v>0</v>
+      </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <v>0</v>
+      </c>
+      <c r="AE16">
+        <v>0</v>
+      </c>
+      <c r="AF16">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="3"/>
+    </row>
+    <row r="17" spans="1:33" ht="15.75" customHeight="1" thickBot="1">
       <c r="A17" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="15.75" customHeight="1" thickBot="1">
+        <v>32</v>
+      </c>
+      <c r="Q17">
+        <v>4</v>
+      </c>
+      <c r="R17">
+        <v>4</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>1</v>
+      </c>
+      <c r="V17">
+        <v>1</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>3</v>
+      </c>
+      <c r="Z17">
+        <v>3</v>
+      </c>
+      <c r="AA17">
+        <v>3</v>
+      </c>
+      <c r="AB17">
+        <v>0</v>
+      </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <v>0</v>
+      </c>
+      <c r="AE17">
+        <v>0</v>
+      </c>
+      <c r="AF17">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="3"/>
+    </row>
+    <row r="18" spans="1:33" ht="15.75" customHeight="1" thickBot="1">
       <c r="A18" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A19" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A20" s="2" t="s">
-        <v>15</v>
+      <c r="R18">
+        <v>4</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>1</v>
+      </c>
+      <c r="V18">
+        <v>1</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <v>3</v>
+      </c>
+      <c r="Z18">
+        <v>3</v>
+      </c>
+      <c r="AA18">
+        <v>3</v>
+      </c>
+      <c r="AB18">
+        <v>0</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
+      <c r="AE18">
+        <v>0</v>
+      </c>
+      <c r="AF18">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="3"/>
+    </row>
+    <row r="19" spans="1:33" ht="15.75" customHeight="1">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="S19">
+        <v>4</v>
+      </c>
+      <c r="T19">
+        <v>4</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
+      <c r="AB19">
+        <v>0</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AE19">
+        <v>0</v>
+      </c>
+      <c r="AF19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" ht="15.75" customHeight="1">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="T20">
+        <v>4</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20">
+        <v>0</v>
+      </c>
+      <c r="Z20">
+        <v>0</v>
+      </c>
+      <c r="AA20">
+        <v>0</v>
+      </c>
+      <c r="AB20">
+        <v>0</v>
+      </c>
+      <c r="AC20">
+        <v>0</v>
+      </c>
+      <c r="AD20">
+        <v>0</v>
+      </c>
+      <c r="AE20">
+        <v>0</v>
+      </c>
+      <c r="AF20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" ht="15.75" customHeight="1">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="U21">
+        <v>4</v>
+      </c>
+      <c r="V21">
+        <v>4</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <v>0</v>
+      </c>
+      <c r="AA21">
+        <v>0</v>
+      </c>
+      <c r="AB21">
+        <v>0</v>
+      </c>
+      <c r="AC21">
+        <v>0</v>
+      </c>
+      <c r="AD21">
+        <v>0</v>
+      </c>
+      <c r="AE21">
+        <v>0</v>
+      </c>
+      <c r="AF21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" ht="15.75" customHeight="1">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="V22">
+        <v>4</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+      <c r="Y22">
+        <v>0</v>
+      </c>
+      <c r="Z22">
+        <v>0</v>
+      </c>
+      <c r="AA22">
+        <v>0</v>
+      </c>
+      <c r="AB22">
+        <v>0</v>
+      </c>
+      <c r="AC22">
+        <v>0</v>
+      </c>
+      <c r="AD22">
+        <v>0</v>
+      </c>
+      <c r="AE22">
+        <v>0</v>
+      </c>
+      <c r="AF22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" ht="15.75" customHeight="1">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="W23">
+        <v>4</v>
+      </c>
+      <c r="X23">
+        <v>4</v>
+      </c>
+      <c r="Y23">
+        <v>0</v>
+      </c>
+      <c r="Z23">
+        <v>0</v>
+      </c>
+      <c r="AA23">
+        <v>0</v>
+      </c>
+      <c r="AB23">
+        <v>0</v>
+      </c>
+      <c r="AC23">
+        <v>0</v>
+      </c>
+      <c r="AD23">
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" ht="15.75" customHeight="1">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="X24">
+        <v>4</v>
+      </c>
+      <c r="Y24">
+        <v>0</v>
+      </c>
+      <c r="Z24">
+        <v>0</v>
+      </c>
+      <c r="AA24">
+        <v>0</v>
+      </c>
+      <c r="AB24">
+        <v>0</v>
+      </c>
+      <c r="AC24">
+        <v>0</v>
+      </c>
+      <c r="AD24">
+        <v>0</v>
+      </c>
+      <c r="AE24">
+        <v>0</v>
+      </c>
+      <c r="AF24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" ht="15.75" customHeight="1">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y25">
+        <v>4</v>
+      </c>
+      <c r="Z25">
+        <v>4</v>
+      </c>
+      <c r="AA25">
+        <v>4</v>
+      </c>
+      <c r="AB25">
+        <v>0</v>
+      </c>
+      <c r="AC25">
+        <v>0</v>
+      </c>
+      <c r="AD25">
+        <v>0</v>
+      </c>
+      <c r="AE25">
+        <v>0</v>
+      </c>
+      <c r="AF25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" ht="15.75" customHeight="1">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z26">
+        <v>4</v>
+      </c>
+      <c r="AA26">
+        <v>4</v>
+      </c>
+      <c r="AB26">
+        <v>0</v>
+      </c>
+      <c r="AC26">
+        <v>0</v>
+      </c>
+      <c r="AD26">
+        <v>0</v>
+      </c>
+      <c r="AE26">
+        <v>0</v>
+      </c>
+      <c r="AF26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" ht="15.75" customHeight="1">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA27">
+        <v>4</v>
+      </c>
+      <c r="AB27">
+        <v>0</v>
+      </c>
+      <c r="AC27">
+        <v>0</v>
+      </c>
+      <c r="AD27">
+        <v>0</v>
+      </c>
+      <c r="AE27">
+        <v>0</v>
+      </c>
+      <c r="AF27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" ht="15.75" customHeight="1">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB28">
+        <v>4</v>
+      </c>
+      <c r="AC28">
+        <v>4</v>
+      </c>
+      <c r="AD28">
+        <v>4</v>
+      </c>
+      <c r="AE28">
+        <v>0</v>
+      </c>
+      <c r="AF28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" ht="15.75" customHeight="1">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC29">
+        <v>4</v>
+      </c>
+      <c r="AD29">
+        <v>4</v>
+      </c>
+      <c r="AE29">
+        <v>0</v>
+      </c>
+      <c r="AF29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" ht="15.75" customHeight="1">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD30">
+        <v>4</v>
+      </c>
+      <c r="AE30">
+        <v>0</v>
+      </c>
+      <c r="AF30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" ht="15.75" customHeight="1">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE31">
+        <v>4</v>
+      </c>
+      <c r="AF31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" ht="15.75" customHeight="1">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF32">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated song correlation data
</commit_message>
<xml_diff>
--- a/Song Correlation.xlsx
+++ b/Song Correlation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>Alice in Chains - Rooster</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>The Pixies - Where Is My Mind</t>
+  </si>
+  <si>
+    <t>Katy Perry - California Gurls</t>
   </si>
 </sst>
 </file>
@@ -479,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="X19" sqref="X19"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1924,7 +1927,7 @@
     </row>
     <row r="20" spans="1:33" ht="15.75" customHeight="1">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="T20">
         <v>4</v>

</xml_diff>